<commit_message>
Screnshot and Excel Utility Changes
</commit_message>
<xml_diff>
--- a/TestAppProject.xlsx
+++ b/TestAppProject.xlsx
@@ -1,45 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apoorv.r\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0B22130-B1AD-4183-A0A7-7C5EDB5D68E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{8D699E9D-2F5C-4293-A6FA-16B399D9F4E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6A2EAC76-F80F-41F0-BC38-DD43CFF9E3A2}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="20790" windowHeight="11820" xr2:uid="{6A2EAC76-F80F-41F0-BC38-DD43CFF9E3A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>rastogiapoorv17@gmail.com</t>
   </si>
   <si>
     <t>Welcome123</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Credentials</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -402,25 +401,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E9227A5-A449-4F0F-9338-A168DBBE6AD2}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{494AB6D3-8B24-48E9-A7DF-BDADFCA94710}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{494AB6D3-8B24-48E9-A7DF-BDADFCA94710}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>